<commit_message>
Version 2 of The File
</commit_message>
<xml_diff>
--- a/Excel Files/Book1.xlsx
+++ b/Excel Files/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DocumentsRepository\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0078B88F-EE41-4833-80B1-674AFFB0EF7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD41806-1B11-44BB-85BC-8F501D6CB614}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{FA15C3B8-26AE-4B88-858C-B4133CF67B66}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Sr No</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>This is Version 1 of File</t>
+  </si>
+  <si>
+    <t>This is Version 2 of File</t>
   </si>
 </sst>
 </file>
@@ -390,13 +393,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423FCCF3-F2E4-40CA-8459-E02D0660ABCE}">
-  <dimension ref="B4:C5"/>
+  <dimension ref="B4:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -412,6 +418,14 @@
       </c>
       <c r="C5" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 3 of The File Updated
</commit_message>
<xml_diff>
--- a/Excel Files/Book1.xlsx
+++ b/Excel Files/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DocumentsRepository\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD41806-1B11-44BB-85BC-8F501D6CB614}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10520DF-0D9E-4009-8FCF-5F271A4626C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{FA15C3B8-26AE-4B88-858C-B4133CF67B66}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Sr No</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>This is Version 2 of File</t>
+  </si>
+  <si>
+    <t>This is Version 3 of File</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423FCCF3-F2E4-40CA-8459-E02D0660ABCE}">
-  <dimension ref="B4:C6"/>
+  <dimension ref="B4:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,6 +431,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 4 of The File Updated
</commit_message>
<xml_diff>
--- a/Excel Files/Book1.xlsx
+++ b/Excel Files/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DocumentsRepository\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10520DF-0D9E-4009-8FCF-5F271A4626C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9323542C-BEB3-4328-BEA9-2658ABBD7A97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{FA15C3B8-26AE-4B88-858C-B4133CF67B66}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Sr No</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>This is Version 3 of File</t>
+  </si>
+  <si>
+    <t>This is Version 4 of File</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423FCCF3-F2E4-40CA-8459-E02D0660ABCE}">
-  <dimension ref="B4:C7"/>
+  <dimension ref="B4:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +442,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 5 of The File Updated
</commit_message>
<xml_diff>
--- a/Excel Files/Book1.xlsx
+++ b/Excel Files/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DocumentsRepository\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9323542C-BEB3-4328-BEA9-2658ABBD7A97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8226817E-0EF7-43BA-B183-F23C40F7536F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{FA15C3B8-26AE-4B88-858C-B4133CF67B66}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sr No</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>This is Version 4 of File</t>
+  </si>
+  <si>
+    <t>This is Version 5 of File</t>
   </si>
 </sst>
 </file>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423FCCF3-F2E4-40CA-8459-E02D0660ABCE}">
-  <dimension ref="B4:C8"/>
+  <dimension ref="B4:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,6 +453,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>